<commit_message>
Log, email, jpa funcionando, división de paquetes, dependencias y BBDD
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -101,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,18 +425,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -509,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Integracion en master funcionando
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -101,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,18 +425,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -509,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>